<commit_message>
Added Listing Page for All Runes
</commit_message>
<xml_diff>
--- a/Runes/Runes.xlsx
+++ b/Runes/Runes.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jude5\Documents\GitHub\RunicTellers\Runes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F97E8F-6C26-4D12-9BB7-21B51AD518C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21075" windowHeight="8265"/>
+    <workbookView xWindow="7200" yWindow="2085" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,8 +480,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -510,18 +516,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -568,7 +586,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -600,9 +618,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -634,6 +670,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -809,25 +863,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="48" customWidth="1"/>
-    <col min="5" max="5" width="46.5703125" customWidth="1"/>
-    <col min="6" max="6" width="55.7109375" customWidth="1"/>
-    <col min="7" max="7" width="51.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -856,152 +910,152 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="3">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="3">
         <v>2</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="3">
         <v>3</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="3">
         <v>4</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1030,7 +1084,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1059,7 +1113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1088,7 +1142,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1117,7 +1171,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1146,7 +1200,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1175,7 +1229,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1204,7 +1258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1233,7 +1287,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1262,7 +1316,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1291,7 +1345,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1320,7 +1374,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1349,7 +1403,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1378,7 +1432,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1407,7 +1461,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1436,7 +1490,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1465,7 +1519,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1494,7 +1548,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1523,7 +1577,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1554,28 +1608,29 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>